<commit_message>
mongo pass as env
</commit_message>
<xml_diff>
--- a/Student Timetable/FourthYearTimetable.xlsx
+++ b/Student Timetable/FourthYearTimetable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\Exam-Seat-Arrangement\Student Timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F909CBCB-43B6-4DB0-BEB3-9DBAB21E2CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E053765F-59F9-47A9-BADD-513E545F1A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cs" sheetId="1" r:id="rId1"/>
@@ -38,40 +38,40 @@
     <t>date</t>
   </si>
   <si>
-    <t>dc</t>
-  </si>
-  <si>
-    <t>embedded systems</t>
-  </si>
-  <si>
-    <t>electrical system design</t>
-  </si>
-  <si>
-    <t>energy management</t>
-  </si>
-  <si>
-    <t>cable</t>
-  </si>
-  <si>
-    <t>modem</t>
-  </si>
-  <si>
-    <t>cement</t>
-  </si>
-  <si>
-    <t>powder</t>
-  </si>
-  <si>
-    <t>brake</t>
-  </si>
-  <si>
-    <t>engv</t>
-  </si>
-  <si>
-    <t>robmachine</t>
-  </si>
-  <si>
-    <t>armor</t>
+    <t>Dc</t>
+  </si>
+  <si>
+    <t>Embedded systems</t>
+  </si>
+  <si>
+    <t>Control Systems</t>
+  </si>
+  <si>
+    <t>VLSI Design</t>
+  </si>
+  <si>
+    <t>Hydraulics</t>
+  </si>
+  <si>
+    <t>Geomatics</t>
+  </si>
+  <si>
+    <t>Electromagnetic Theory</t>
+  </si>
+  <si>
+    <t>Renewable Energy Sources</t>
+  </si>
+  <si>
+    <t>Theory of Machines</t>
+  </si>
+  <si>
+    <t>Engineering Thermodynamics</t>
+  </si>
+  <si>
+    <t>System Dynamics and Analysis</t>
+  </si>
+  <si>
+    <t>Instrumentation and Measurement</t>
   </si>
 </sst>
 </file>
@@ -393,7 +393,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,7 +435,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +456,7 @@
         <v>44980</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -464,11 +464,12 @@
         <v>44982</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -476,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EAF7968-D6FA-48A8-B8C0-B46DCC721F5B}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +499,7 @@
         <v>44969</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -506,7 +507,7 @@
         <v>44971</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -519,7 +520,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:E6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +542,7 @@
         <v>45040</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -549,7 +550,7 @@
         <v>44982</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -562,7 +563,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,13 +604,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B8B53A5-7236-4BA3-9C70-15AA391447F9}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>